<commit_message>
v1.0.1 P! - Finalizado
</commit_message>
<xml_diff>
--- a/Versoes_Descricao.xlsx
+++ b/Versoes_Descricao.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Versões Sistema</t>
   </si>
@@ -68,7 +68,34 @@
     <t>ok</t>
   </si>
   <si>
-    <t>desenv</t>
+    <t>chekclist</t>
+  </si>
+  <si>
+    <t>Correcao Transacao Cartao</t>
+  </si>
+  <si>
+    <t>Verificar Saldo no Carregamento da tela</t>
+  </si>
+  <si>
+    <t>(-)</t>
+  </si>
+  <si>
+    <t>Melhorias Programacao</t>
+  </si>
+  <si>
+    <t>Erros - Tabela Geral</t>
+  </si>
+  <si>
+    <t>Front-End</t>
+  </si>
+  <si>
+    <t>Menu de Meses - Superior</t>
+  </si>
+  <si>
+    <t>Configuração de Categorias</t>
+  </si>
+  <si>
+    <t>Validar Insert Transacao</t>
   </si>
 </sst>
 </file>
@@ -91,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +128,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -117,8 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -140,8 +181,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G9" totalsRowShown="0">
-  <autoFilter ref="B3:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G17" totalsRowShown="0">
+  <autoFilter ref="B3:G17"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Status"/>
     <tableColumn id="2" name="Principal"/>
@@ -417,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G9"/>
+  <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,14 +474,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -463,7 +504,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4">
@@ -483,27 +524,27 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6">
@@ -523,7 +564,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7">
@@ -543,8 +584,8 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>14</v>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -563,8 +604,8 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>14</v>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -580,6 +621,166 @@
       </c>
       <c r="G9" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1.0.1 P! F - Correcao tela Geral
</commit_message>
<xml_diff>
--- a/Versoes_Descricao.xlsx
+++ b/Versoes_Descricao.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp---\www\Controle_Financeiro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Xampp\htdocs\Testes\Controle_Financeiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,8 +143,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,17 +158,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +481,7 @@
   <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,13 +674,13 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -674,13 +694,13 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -694,13 +714,13 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -717,10 +737,10 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v.1.1.1.0 P! - Verificação a Atualização no Carregamento da Pagina
</commit_message>
<xml_diff>
--- a/Versoes_Descricao.xlsx
+++ b/Versoes_Descricao.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Versões Sistema</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>chekclist</t>
-  </si>
-  <si>
-    <t>Correcao Transacao Cartao</t>
   </si>
   <si>
     <t>Verificar Saldo no Carregamento da tela</t>
@@ -179,10 +176,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,8 +198,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G17" totalsRowShown="0">
-  <autoFilter ref="B3:G17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G16" totalsRowShown="0">
+  <autoFilter ref="B3:G16"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Status"/>
     <tableColumn id="2" name="Principal"/>
@@ -478,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G17"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,14 +491,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -545,7 +542,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -645,42 +642,42 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -694,10 +691,10 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" t="s">
         <v>15</v>
@@ -714,52 +711,52 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -774,33 +771,13 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.3.1.1 Transacao Ok / Alteracao Valor Cartao OK
</commit_message>
<xml_diff>
--- a/Versoes_Descricao.xlsx
+++ b/Versoes_Descricao.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Versões Sistema</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Validar Insert Transacao</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>Dados do Cartao Para Transacao</t>
+  </si>
+  <si>
+    <t>Transacaoes Incertas</t>
   </si>
 </sst>
 </file>
@@ -115,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +155,12 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -172,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -180,6 +195,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,8 +214,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G16" totalsRowShown="0">
-  <autoFilter ref="B3:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G19" totalsRowShown="0">
+  <autoFilter ref="B3:G19"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Status"/>
     <tableColumn id="2" name="Principal"/>
@@ -475,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:G19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,46 +753,102 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.2.3.0 P! - CRUD Transacoes OK
</commit_message>
<xml_diff>
--- a/Versoes_Descricao.xlsx
+++ b/Versoes_Descricao.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Versões Sistema</t>
   </si>
@@ -104,10 +104,19 @@
     <t>Transacaoes Incertas</t>
   </si>
   <si>
-    <t>Multiplas Contas</t>
-  </si>
-  <si>
     <t>Multiplos Cartoes</t>
+  </si>
+  <si>
+    <t>Alterar Transferencia de Contas</t>
+  </si>
+  <si>
+    <t>Js Tela - Controle de Contas</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Multiplas Contas (CRUD Transacoes)</t>
   </si>
 </sst>
 </file>
@@ -213,8 +222,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G21" totalsRowShown="0">
-  <autoFilter ref="B3:G21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G23" totalsRowShown="0">
+  <autoFilter ref="B3:G23"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Status"/>
     <tableColumn id="2" name="Principal"/>
@@ -490,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G21"/>
+  <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,7 +805,9 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C17">
         <v>1</v>
       </c>
@@ -810,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -822,72 +833,108 @@
         <v>2</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
         <v>3</v>
       </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>3</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>14</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.2.3.1 P! - Js e CSS das Contas OK
</commit_message>
<xml_diff>
--- a/Versoes_Descricao.xlsx
+++ b/Versoes_Descricao.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Versões Sistema</t>
   </si>
@@ -502,7 +502,7 @@
   <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,9 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C18">
         <v>1</v>
       </c>
@@ -839,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -857,7 +859,7 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v1.2.3.2 Ok - Alterar Transf Entre Contas
</commit_message>
<xml_diff>
--- a/Versoes_Descricao.xlsx
+++ b/Versoes_Descricao.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Versões Sistema</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Multiplas Contas (CRUD Transacoes)</t>
+  </si>
+  <si>
+    <t>Transf entre contas, contabilizar</t>
   </si>
 </sst>
 </file>
@@ -222,8 +225,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G23" totalsRowShown="0">
-  <autoFilter ref="B3:G23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G24" totalsRowShown="0">
+  <autoFilter ref="B3:G24"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Status"/>
     <tableColumn id="2" name="Principal"/>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G23"/>
+  <dimension ref="B2:G24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +848,9 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C19">
         <v>1</v>
       </c>
@@ -871,53 +876,51 @@
         <v>2</v>
       </c>
       <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
         <v>4</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
         <v>3</v>
       </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -931,12 +934,32 @@
         <v>3</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.2.3.3 Ok - Contabilizacao
</commit_message>
<xml_diff>
--- a/Versoes_Descricao.xlsx
+++ b/Versoes_Descricao.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Versões Sistema</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Transf entre contas, contabilizar</t>
+  </si>
+  <si>
+    <t>Versão Produção (Arrumar Inconsistencias)</t>
   </si>
 </sst>
 </file>
@@ -225,8 +228,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G24" totalsRowShown="0">
-  <autoFilter ref="B3:G24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B3:G25" totalsRowShown="0">
+  <autoFilter ref="B3:G25"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Status"/>
     <tableColumn id="2" name="Principal"/>
@@ -502,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G24"/>
+  <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +871,9 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C20">
         <v>1</v>
       </c>
@@ -904,43 +909,41 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
         <v>3</v>
       </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -954,12 +957,32 @@
         <v>3</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>